<commit_message>
Sửa file Excel và nâng cấp bag
</commit_message>
<xml_diff>
--- a/N65_Happy_Lunch.xlsx
+++ b/N65_Happy_Lunch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apk\git\Happy_Lunch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF7DE69-1813-47D8-8843-3B2D310AEE3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C17C9C-A6F2-4576-8819-E3E17674C6EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2" xr2:uid="{BC20BD91-CA0E-4BED-9EF6-F680DC379E66}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>STT</t>
   </si>
@@ -201,21 +201,12 @@
     <t>Class Diagram</t>
   </si>
   <si>
-    <t>25/03</t>
-  </si>
-  <si>
-    <t>26/03</t>
-  </si>
-  <si>
     <t>2 layout</t>
   </si>
   <si>
     <t>Ít thời gian</t>
   </si>
   <si>
-    <t>28/03</t>
-  </si>
-  <si>
     <t>30/03</t>
   </si>
   <si>
@@ -262,6 +253,33 @@
   </si>
   <si>
     <t>giao diện profile</t>
+  </si>
+  <si>
+    <t>28/03/2019</t>
+  </si>
+  <si>
+    <t>25/03/2019</t>
+  </si>
+  <si>
+    <t>26/03/2019</t>
+  </si>
+  <si>
+    <t>30/03/2019</t>
+  </si>
+  <si>
+    <t>Giao diện home</t>
+  </si>
+  <si>
+    <t>Giao diện admin</t>
+  </si>
+  <si>
+    <t>Giao diện tạo tài khoản</t>
+  </si>
+  <si>
+    <t>Nâng cấp giao diện thông tin món ăn</t>
+  </si>
+  <si>
+    <t>Nâng cấp giao diện profile</t>
   </si>
 </sst>
 </file>
@@ -271,7 +289,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +358,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -361,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -729,12 +754,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -760,19 +823,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -782,12 +832,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -806,6 +850,29 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,13 +891,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,13 +909,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -869,10 +936,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -890,22 +957,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1220,7 +1297,7 @@
   <dimension ref="B3:H14"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1237,22 +1314,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
     </row>
     <row r="6" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="2:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -1297,7 +1374,7 @@
       <c r="G8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="24" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1360,7 +1437,7 @@
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="26" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="7" t="s">
@@ -1383,23 +1460,23 @@
       <c r="E12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="22" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F13" s="30">
+      <c r="F13" s="21">
         <v>398321782</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F14" s="30">
+      <c r="F14" s="21">
         <v>972903907</v>
       </c>
     </row>
@@ -1449,47 +1526,47 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
+      <c r="C7" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
     </row>
     <row r="8" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1501,65 +1578,65 @@
       <c r="G9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="28"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="42">
+      <c r="B10" s="31">
         <v>1</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="44" t="s">
+      <c r="C10" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="46" t="s">
+      <c r="F10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="35" t="s">
         <v>49</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="42">
+      <c r="B11" s="31">
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="36" t="s">
-        <v>74</v>
+      <c r="F11" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="29"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="42">
+      <c r="B12" s="31">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="36" t="s">
-        <v>66</v>
+      <c r="F12" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>49</v>
@@ -1567,20 +1644,20 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="43">
+      <c r="B13" s="32">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>49</v>
@@ -1588,20 +1665,20 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="42">
+      <c r="B14" s="31">
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>67</v>
+      <c r="F14" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>49</v>
@@ -1789,52 +1866,52 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" s="41"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38" s="41"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" s="41"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B40" s="41"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" s="41"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B42" s="41"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1854,671 +1931,683 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132B7DB0-6F4F-4CEE-9902-9AD47C1183AE}">
   <dimension ref="A3:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="75" t="s">
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="79" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="69"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="24" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="76"/>
+      <c r="I8" s="80"/>
     </row>
     <row r="9" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="38"/>
+      <c r="I9" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="82"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="H10" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="37">
+      <c r="I10" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="60"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="37">
+    <row r="11" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="82"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="60"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22" t="s">
+    <row r="12" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="82"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="37">
+      <c r="H12" s="39"/>
+      <c r="I12" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="60"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22" t="s">
+    <row r="13" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="83"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="61"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="37">
+      <c r="H13" s="40"/>
+      <c r="I13" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="26" t="s">
+      <c r="B14" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="38">
+      <c r="F14" s="41"/>
+      <c r="G14" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="41"/>
+      <c r="I14" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="19" t="s">
+      <c r="B15" s="58"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="38">
+      <c r="F15" s="42"/>
+      <c r="G15" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="42"/>
+      <c r="I15" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="B16" s="58"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="38">
+      <c r="F16" s="42"/>
+      <c r="G16" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="42"/>
+      <c r="I16" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="19" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="38">
+      <c r="F17" s="42"/>
+      <c r="G17" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="27" t="s">
+      <c r="B18" s="59"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="43"/>
+      <c r="G18" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="38">
+      <c r="H18" s="43"/>
+      <c r="I18" s="47">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21" t="s">
+      <c r="B19" s="63">
+        <v>43712</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="46"/>
     </row>
     <row r="20" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22" t="s">
+      <c r="B20" s="64"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="37"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="46"/>
     </row>
     <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="37"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="46"/>
     </row>
     <row r="22" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="37"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="46"/>
     </row>
     <row r="23" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23" t="s">
+      <c r="B23" s="65"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="37"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="46"/>
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26" t="s">
+      <c r="B24" s="57"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="38"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="47"/>
     </row>
     <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19" t="s">
+      <c r="B25" s="58"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="38"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="47"/>
     </row>
     <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="s">
+      <c r="B26" s="58"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="38"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="47"/>
     </row>
     <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="s">
+      <c r="B27" s="58"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="38"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20" t="s">
+      <c r="B28" s="84"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="38"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="47"/>
     </row>
     <row r="29" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21" t="s">
+      <c r="B29" s="81"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22" t="s">
+      <c r="B30" s="82"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="37"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22" t="s">
+      <c r="B31" s="82"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="37"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="46"/>
     </row>
     <row r="32" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22" t="s">
+      <c r="B32" s="82"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="37"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23" t="s">
+      <c r="B33" s="83"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="37"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="46"/>
     </row>
     <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26" t="s">
+      <c r="B34" s="57"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="38"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="47"/>
     </row>
     <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19" t="s">
+      <c r="B35" s="58"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="38"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19" t="s">
+      <c r="B36" s="58"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="38"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="47"/>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19" t="s">
+      <c r="B37" s="58"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="38"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="47"/>
     </row>
     <row r="38" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1"/>
-      <c r="B38" s="77"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20" t="s">
+      <c r="B38" s="84"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="38"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="47"/>
     </row>
     <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="I39" s="48"/>
     </row>
     <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="I40" s="48"/>
     </row>
     <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="I41" s="48"/>
     </row>
     <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="I42" s="48"/>
     </row>
     <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="I43" s="48"/>
     </row>
     <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="B44" s="50"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
+      <c r="I44" s="48"/>
     </row>
     <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="B45" s="50"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
+      <c r="I45" s="48"/>
     </row>
     <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
+      <c r="I46" s="48"/>
     </row>
     <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="B47" s="50"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
+      <c r="I47" s="48"/>
     </row>
     <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="B49" s="50"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+      <c r="I49" s="48"/>
     </row>
     <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="I50" s="48"/>
     </row>
     <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D51" s="1"/>
@@ -2526,7 +2615,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="I51" s="48"/>
     </row>
     <row r="52" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D52" s="1"/>
@@ -2534,7 +2623,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
+      <c r="I52" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>

<commit_message>
Update giao diện item của admin
</commit_message>
<xml_diff>
--- a/N65_Happy_Lunch.xlsx
+++ b/N65_Happy_Lunch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apk\git\Happy_Lunch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAC1345-C946-4999-9854-C413E6B8F954}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3821C192-E8CC-4E5C-9B69-FD5F782E7A08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="8376" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="107">
   <si>
     <t>NHÓM 65: HAPPY LUNCH</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>Giao diện thêm item admin</t>
+  </si>
+  <si>
+    <t>16/4</t>
+  </si>
+  <si>
+    <t>19/4</t>
   </si>
 </sst>
 </file>
@@ -1010,6 +1016,99 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1019,101 +1118,8 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2122,7 +2128,7 @@
   <dimension ref="A3:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2140,56 +2146,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="25.8">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
     </row>
     <row r="5" spans="1:9" ht="21">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="7" spans="1:9" ht="18">
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="93"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="103" t="s">
+      <c r="G7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="89" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18">
-      <c r="B8" s="96"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="102"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="48" t="s">
         <v>60</v>
       </c>
@@ -2199,13 +2205,13 @@
       <c r="H8" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="104"/>
+      <c r="I8" s="90"/>
     </row>
     <row r="9" spans="1:9" ht="18">
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D9" s="50" t="s">
@@ -2224,8 +2230,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18">
-      <c r="B10" s="87"/>
-      <c r="C10" s="74"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="83"/>
       <c r="D10" s="52" t="s">
         <v>65</v>
       </c>
@@ -2244,8 +2250,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18">
-      <c r="B11" s="87"/>
-      <c r="C11" s="74"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="52" t="s">
         <v>68</v>
       </c>
@@ -2262,8 +2268,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18">
-      <c r="B12" s="87"/>
-      <c r="C12" s="74"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="52" t="s">
         <v>70</v>
       </c>
@@ -2280,8 +2286,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.600000000000001" thickBot="1">
-      <c r="B13" s="88"/>
-      <c r="C13" s="75"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="53" t="s">
         <v>71</v>
       </c>
@@ -2299,10 +2305,10 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
       <c r="A14" s="54"/>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="101" t="s">
         <v>95</v>
       </c>
       <c r="D14" s="55" t="s">
@@ -2322,8 +2328,8 @@
     </row>
     <row r="15" spans="1:9" ht="18">
       <c r="A15" s="54"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="102"/>
       <c r="D15" s="57" t="s">
         <v>74</v>
       </c>
@@ -2341,8 +2347,8 @@
     </row>
     <row r="16" spans="1:9" ht="18">
       <c r="A16" s="54"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="71"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="102"/>
       <c r="D16" s="57" t="s">
         <v>50</v>
       </c>
@@ -2360,8 +2366,8 @@
     </row>
     <row r="17" spans="1:9" ht="18">
       <c r="A17" s="54"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="71"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="102"/>
       <c r="D17" s="57" t="s">
         <v>48</v>
       </c>
@@ -2379,8 +2385,8 @@
     </row>
     <row r="18" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A18" s="54"/>
-      <c r="B18" s="79"/>
-      <c r="C18" s="72"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="58" t="s">
         <v>52</v>
       </c>
@@ -2398,10 +2404,10 @@
     </row>
     <row r="19" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="54"/>
-      <c r="B19" s="80">
+      <c r="B19" s="94">
         <v>43712</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="82" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="50" t="s">
@@ -2421,8 +2427,8 @@
     </row>
     <row r="20" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A20" s="54"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="74"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="52" t="s">
         <v>76</v>
       </c>
@@ -2440,8 +2446,8 @@
     </row>
     <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A21" s="54"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="74"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="83"/>
       <c r="D21" s="52" t="s">
         <v>77</v>
       </c>
@@ -2459,8 +2465,8 @@
     </row>
     <row r="22" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A22" s="54"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="74"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="83"/>
       <c r="D22" s="52" t="s">
         <v>78</v>
       </c>
@@ -2478,8 +2484,8 @@
     </row>
     <row r="23" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A23" s="54"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="75"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="84"/>
       <c r="D23" s="53" t="s">
         <v>79</v>
       </c>
@@ -2497,8 +2503,12 @@
     </row>
     <row r="24" spans="1:9" ht="18">
       <c r="A24" s="54"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="97" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="101" t="s">
+        <v>106</v>
+      </c>
       <c r="D24" s="55" t="s">
         <v>100</v>
       </c>
@@ -2512,8 +2522,8 @@
     </row>
     <row r="25" spans="1:9" ht="18">
       <c r="A25" s="54"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="71"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="102"/>
       <c r="D25" s="57" t="s">
         <v>104</v>
       </c>
@@ -2527,8 +2537,8 @@
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="A26" s="54"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="71"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="102"/>
       <c r="D26" s="57" t="s">
         <v>101</v>
       </c>
@@ -2542,8 +2552,8 @@
     </row>
     <row r="27" spans="1:9" ht="18">
       <c r="A27" s="54"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="71"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="102"/>
       <c r="D27" s="57" t="s">
         <v>102</v>
       </c>
@@ -2557,8 +2567,8 @@
     </row>
     <row r="28" spans="1:9" ht="18">
       <c r="A28" s="54"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="76"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="59" t="s">
         <v>103</v>
       </c>
@@ -2572,8 +2582,8 @@
     </row>
     <row r="29" spans="1:9" ht="18">
       <c r="A29" s="54"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="73"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="82"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50" t="s">
         <v>9</v>
@@ -2585,8 +2595,8 @@
     </row>
     <row r="30" spans="1:9" ht="18">
       <c r="A30" s="54"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="74"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="52"/>
       <c r="E30" s="52" t="s">
         <v>14</v>
@@ -2598,8 +2608,8 @@
     </row>
     <row r="31" spans="1:9" ht="18">
       <c r="A31" s="54"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="74"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="52"/>
       <c r="E31" s="52" t="s">
         <v>19</v>
@@ -2611,8 +2621,8 @@
     </row>
     <row r="32" spans="1:9" ht="18">
       <c r="A32" s="54"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="74"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="52"/>
       <c r="E32" s="52" t="s">
         <v>24</v>
@@ -2624,8 +2634,8 @@
     </row>
     <row r="33" spans="1:9" ht="18">
       <c r="A33" s="54"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="75"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="84"/>
       <c r="D33" s="53"/>
       <c r="E33" s="53" t="s">
         <v>29</v>
@@ -2637,8 +2647,8 @@
     </row>
     <row r="34" spans="1:9" ht="18">
       <c r="A34" s="54"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="70"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="101"/>
       <c r="D34" s="55"/>
       <c r="E34" s="55" t="s">
         <v>9</v>
@@ -2650,8 +2660,8 @@
     </row>
     <row r="35" spans="1:9" ht="18">
       <c r="A35" s="54"/>
-      <c r="B35" s="84"/>
-      <c r="C35" s="71"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="102"/>
       <c r="D35" s="57"/>
       <c r="E35" s="57" t="s">
         <v>14</v>
@@ -2663,8 +2673,8 @@
     </row>
     <row r="36" spans="1:9" ht="18">
       <c r="A36" s="54"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="71"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="102"/>
       <c r="D36" s="57"/>
       <c r="E36" s="57" t="s">
         <v>19</v>
@@ -2676,8 +2686,8 @@
     </row>
     <row r="37" spans="1:9" ht="18">
       <c r="A37" s="54"/>
-      <c r="B37" s="84"/>
-      <c r="C37" s="71"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="102"/>
       <c r="D37" s="57"/>
       <c r="E37" s="57" t="s">
         <v>24</v>
@@ -2689,8 +2699,8 @@
     </row>
     <row r="38" spans="1:9" ht="18">
       <c r="A38" s="54"/>
-      <c r="B38" s="85"/>
-      <c r="C38" s="76"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="104"/>
       <c r="D38" s="59"/>
       <c r="E38" s="59" t="s">
         <v>29</v>
@@ -2850,6 +2860,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B34:B38"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="F7:H7"/>
@@ -2860,16 +2880,6 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C38"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Ghép code giao diện cá nhân vào
Đã hoàn tất ghép code giao diện cá nhân vào
</commit_message>
<xml_diff>
--- a/N65_Happy_Lunch.xlsx
+++ b/N65_Happy_Lunch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apk\git\Happy_Lunch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3821C192-E8CC-4E5C-9B69-FD5F782E7A08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9047765-789F-4868-A912-D53D5E8F27FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="8376" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="8376" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="117">
   <si>
     <t>NHÓM 65: HAPPY LUNCH</t>
   </si>
@@ -344,6 +344,36 @@
   </si>
   <si>
     <t>19/4</t>
+  </si>
+  <si>
+    <t>Giao diện item của admin</t>
+  </si>
+  <si>
+    <t>nâng cấp giao diện item của admin</t>
+  </si>
+  <si>
+    <t>kết nối tài khoản với firebase</t>
+  </si>
+  <si>
+    <t>Kết nối tài khoản với firebase</t>
+  </si>
+  <si>
+    <t>firebase</t>
+  </si>
+  <si>
+    <t>Firebase</t>
+  </si>
+  <si>
+    <t>giao diện setting</t>
+  </si>
+  <si>
+    <t>Giao diện setting</t>
+  </si>
+  <si>
+    <t>nâng cấp giao diện profile</t>
+  </si>
+  <si>
+    <t>giao diện home của admin</t>
   </si>
 </sst>
 </file>
@@ -1016,6 +1046,66 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1037,30 +1127,12 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1078,48 +1150,6 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1614,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -1935,59 +1965,121 @@
       <c r="B22" s="16">
         <v>13</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="14"/>
+      <c r="C22" s="40">
+        <v>43575</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="8">
         <v>14</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="C23" s="40">
+        <v>43575</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="8">
         <v>15</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="C24" s="40">
+        <v>43575</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="16">
         <v>16</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="C25" s="40">
+        <v>43576</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="8">
         <v>17</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="C26" s="40">
+        <v>43576</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="12"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="B27" s="8">
+        <v>18</v>
+      </c>
+      <c r="C27" s="40">
+        <v>43576</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" s="12"/>
@@ -2127,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2146,56 +2238,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="25.8">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
     </row>
     <row r="5" spans="1:9" ht="21">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
     </row>
     <row r="7" spans="1:9" ht="18">
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="89" t="s">
+      <c r="G7" s="93"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="103" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18">
-      <c r="B8" s="76"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="88"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="102"/>
       <c r="F8" s="48" t="s">
         <v>60</v>
       </c>
@@ -2205,13 +2297,13 @@
       <c r="H8" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="90"/>
+      <c r="I8" s="104"/>
     </row>
     <row r="9" spans="1:9" ht="18">
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="73" t="s">
         <v>96</v>
       </c>
       <c r="D9" s="50" t="s">
@@ -2230,8 +2322,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18">
-      <c r="B10" s="78"/>
-      <c r="C10" s="83"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="74"/>
       <c r="D10" s="52" t="s">
         <v>65</v>
       </c>
@@ -2250,8 +2342,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18">
-      <c r="B11" s="78"/>
-      <c r="C11" s="83"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="52" t="s">
         <v>68</v>
       </c>
@@ -2268,8 +2360,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18">
-      <c r="B12" s="78"/>
-      <c r="C12" s="83"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="52" t="s">
         <v>70</v>
       </c>
@@ -2286,8 +2378,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.600000000000001" thickBot="1">
-      <c r="B13" s="79"/>
-      <c r="C13" s="84"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="53" t="s">
         <v>71</v>
       </c>
@@ -2305,10 +2397,10 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
       <c r="A14" s="54"/>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="101" t="s">
+      <c r="C14" s="70" t="s">
         <v>95</v>
       </c>
       <c r="D14" s="55" t="s">
@@ -2328,8 +2420,8 @@
     </row>
     <row r="15" spans="1:9" ht="18">
       <c r="A15" s="54"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="102"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="57" t="s">
         <v>74</v>
       </c>
@@ -2347,8 +2439,8 @@
     </row>
     <row r="16" spans="1:9" ht="18">
       <c r="A16" s="54"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="102"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="57" t="s">
         <v>50</v>
       </c>
@@ -2366,8 +2458,8 @@
     </row>
     <row r="17" spans="1:9" ht="18">
       <c r="A17" s="54"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="102"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="57" t="s">
         <v>48</v>
       </c>
@@ -2385,8 +2477,8 @@
     </row>
     <row r="18" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A18" s="54"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="103"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="58" t="s">
         <v>52</v>
       </c>
@@ -2404,10 +2496,10 @@
     </row>
     <row r="19" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="54"/>
-      <c r="B19" s="94">
+      <c r="B19" s="80">
         <v>43712</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="73" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="50" t="s">
@@ -2427,8 +2519,8 @@
     </row>
     <row r="20" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A20" s="54"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="83"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="52" t="s">
         <v>76</v>
       </c>
@@ -2446,8 +2538,8 @@
     </row>
     <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A21" s="54"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="83"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="52" t="s">
         <v>77</v>
       </c>
@@ -2465,8 +2557,8 @@
     </row>
     <row r="22" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A22" s="54"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="83"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="52" t="s">
         <v>78</v>
       </c>
@@ -2484,8 +2576,8 @@
     </row>
     <row r="23" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A23" s="54"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="84"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="75"/>
       <c r="D23" s="53" t="s">
         <v>79</v>
       </c>
@@ -2503,10 +2595,10 @@
     </row>
     <row r="24" spans="1:9" ht="18">
       <c r="A24" s="54"/>
-      <c r="B24" s="97" t="s">
+      <c r="B24" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="70" t="s">
         <v>106</v>
       </c>
       <c r="D24" s="55" t="s">
@@ -2516,14 +2608,18 @@
         <v>9</v>
       </c>
       <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
+      <c r="G24" s="55" t="s">
+        <v>73</v>
+      </c>
       <c r="H24" s="55"/>
-      <c r="I24" s="56"/>
+      <c r="I24" s="56">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="18">
       <c r="A25" s="54"/>
-      <c r="B25" s="98"/>
-      <c r="C25" s="102"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="57" t="s">
         <v>104</v>
       </c>
@@ -2531,14 +2627,18 @@
         <v>14</v>
       </c>
       <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
+      <c r="G25" s="57" t="s">
+        <v>73</v>
+      </c>
       <c r="H25" s="57"/>
-      <c r="I25" s="56"/>
+      <c r="I25" s="56">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="A26" s="54"/>
-      <c r="B26" s="98"/>
-      <c r="C26" s="102"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="57" t="s">
         <v>101</v>
       </c>
@@ -2546,29 +2646,37 @@
         <v>19</v>
       </c>
       <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
+      <c r="G26" s="57" t="s">
+        <v>73</v>
+      </c>
       <c r="H26" s="57"/>
-      <c r="I26" s="56"/>
+      <c r="I26" s="56">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="18">
       <c r="A27" s="54"/>
-      <c r="B27" s="98"/>
-      <c r="C27" s="102"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="57" t="s">
         <v>102</v>
       </c>
       <c r="E27" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="57"/>
+      <c r="F27" s="57" t="s">
+        <v>98</v>
+      </c>
       <c r="G27" s="57"/>
       <c r="H27" s="57"/>
-      <c r="I27" s="56"/>
+      <c r="I27" s="56">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="18">
       <c r="A28" s="54"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="104"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="76"/>
       <c r="D28" s="59" t="s">
         <v>103</v>
       </c>
@@ -2576,14 +2684,18 @@
         <v>29</v>
       </c>
       <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
+      <c r="G28" s="59" t="s">
+        <v>73</v>
+      </c>
       <c r="H28" s="59"/>
-      <c r="I28" s="56"/>
+      <c r="I28" s="56">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="18">
       <c r="A29" s="54"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="82"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="73"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50" t="s">
         <v>9</v>
@@ -2595,8 +2707,8 @@
     </row>
     <row r="30" spans="1:9" ht="18">
       <c r="A30" s="54"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="83"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="74"/>
       <c r="D30" s="52"/>
       <c r="E30" s="52" t="s">
         <v>14</v>
@@ -2608,8 +2720,8 @@
     </row>
     <row r="31" spans="1:9" ht="18">
       <c r="A31" s="54"/>
-      <c r="B31" s="78"/>
-      <c r="C31" s="83"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="52"/>
       <c r="E31" s="52" t="s">
         <v>19</v>
@@ -2621,8 +2733,8 @@
     </row>
     <row r="32" spans="1:9" ht="18">
       <c r="A32" s="54"/>
-      <c r="B32" s="78"/>
-      <c r="C32" s="83"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="74"/>
       <c r="D32" s="52"/>
       <c r="E32" s="52" t="s">
         <v>24</v>
@@ -2634,8 +2746,8 @@
     </row>
     <row r="33" spans="1:9" ht="18">
       <c r="A33" s="54"/>
-      <c r="B33" s="79"/>
-      <c r="C33" s="84"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="75"/>
       <c r="D33" s="53"/>
       <c r="E33" s="53" t="s">
         <v>29</v>
@@ -2647,8 +2759,8 @@
     </row>
     <row r="34" spans="1:9" ht="18">
       <c r="A34" s="54"/>
-      <c r="B34" s="100"/>
-      <c r="C34" s="101"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="70"/>
       <c r="D34" s="55"/>
       <c r="E34" s="55" t="s">
         <v>9</v>
@@ -2660,8 +2772,8 @@
     </row>
     <row r="35" spans="1:9" ht="18">
       <c r="A35" s="54"/>
-      <c r="B35" s="98"/>
-      <c r="C35" s="102"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="71"/>
       <c r="D35" s="57"/>
       <c r="E35" s="57" t="s">
         <v>14</v>
@@ -2673,8 +2785,8 @@
     </row>
     <row r="36" spans="1:9" ht="18">
       <c r="A36" s="54"/>
-      <c r="B36" s="98"/>
-      <c r="C36" s="102"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="71"/>
       <c r="D36" s="57"/>
       <c r="E36" s="57" t="s">
         <v>19</v>
@@ -2686,8 +2798,8 @@
     </row>
     <row r="37" spans="1:9" ht="18">
       <c r="A37" s="54"/>
-      <c r="B37" s="98"/>
-      <c r="C37" s="102"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="71"/>
       <c r="D37" s="57"/>
       <c r="E37" s="57" t="s">
         <v>24</v>
@@ -2699,8 +2811,8 @@
     </row>
     <row r="38" spans="1:9" ht="18">
       <c r="A38" s="54"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="104"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="76"/>
       <c r="D38" s="59"/>
       <c r="E38" s="59" t="s">
         <v>29</v>
@@ -2860,16 +2972,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B34:B38"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="F7:H7"/>
@@ -2880,6 +2982,16 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C38"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>